<commit_message>
versao Tassio e Tiago unidas
</commit_message>
<xml_diff>
--- a/Arquivos/Dataset/related queries/relatedQueries_ginasio.xlsx
+++ b/Arquivos/Dataset/related queries/relatedQueries_ginasio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projeto PP\GymTrend-Task-Force\Arquivos\Dataset\related queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE714C1D-5714-4B02-A912-FAE5AADED2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056DFC5B-B34B-4544-9BC0-D7EBC16B17C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOP" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>element ginasio</t>
   </si>
@@ -105,6 +105,123 @@
   </si>
   <si>
     <t>Valor</t>
+  </si>
+  <si>
+    <t>ginasio</t>
+  </si>
+  <si>
+    <t>element ginásio</t>
+  </si>
+  <si>
+    <t>ginásio lisboa</t>
+  </si>
+  <si>
+    <t>ginásio fitness hut</t>
+  </si>
+  <si>
+    <t>ginásio perto de mim</t>
+  </si>
+  <si>
+    <t>ginásios</t>
+  </si>
+  <si>
+    <t>supera</t>
+  </si>
+  <si>
+    <t>ginásio venda nova</t>
+  </si>
+  <si>
+    <t>rpm</t>
+  </si>
+  <si>
+    <t>ginásio element odivelas</t>
+  </si>
+  <si>
+    <t>ginásio clube portugues</t>
+  </si>
+  <si>
+    <t>ginasios coimbra</t>
+  </si>
+  <si>
+    <t>ginasio clube portugues</t>
+  </si>
+  <si>
+    <t>body balance</t>
+  </si>
+  <si>
+    <t>solinca</t>
+  </si>
+  <si>
+    <t>ginasios lisboa</t>
+  </si>
+  <si>
+    <t>fitness hut</t>
+  </si>
+  <si>
+    <t>ginasios porto</t>
+  </si>
+  <si>
+    <t>fitness up</t>
+  </si>
+  <si>
+    <t>holmes place</t>
+  </si>
+  <si>
+    <t>ginasios gaia</t>
+  </si>
+  <si>
+    <t>ginasios braga</t>
+  </si>
+  <si>
+    <t>ginasios perto de mim</t>
+  </si>
+  <si>
+    <t>jp ginasios</t>
+  </si>
+  <si>
+    <t>ginasios portugal</t>
+  </si>
+  <si>
+    <t>ginasios aveiro</t>
+  </si>
+  <si>
+    <t>ginasios leiria</t>
+  </si>
+  <si>
+    <t>ginasios almada</t>
+  </si>
+  <si>
+    <t>ginasios setubal</t>
+  </si>
+  <si>
+    <t>ginasios funchal</t>
+  </si>
+  <si>
+    <t>solinca preços</t>
+  </si>
+  <si>
+    <t>ginasios odivelas</t>
+  </si>
+  <si>
+    <t>ginasios em lisboa</t>
+  </si>
+  <si>
+    <t>ginasios oeiras</t>
+  </si>
+  <si>
+    <t>holmes place preços</t>
+  </si>
+  <si>
+    <t>fitness hut leiria</t>
+  </si>
+  <si>
+    <t>ginásios lisboa</t>
+  </si>
+  <si>
+    <t>ginásios porto</t>
+  </si>
+  <si>
+    <t>ginásios perto de mim</t>
   </si>
 </sst>
 </file>
@@ -946,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1165,6 +1282,390 @@
         <v>2</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>64</v>
+      </c>
+      <c r="B69">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>62</v>
+      </c>
+      <c r="B74">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1174,7 +1675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>

</xml_diff>